<commit_message>
Profile & ID removed from POM Files to execute mutiple tests
</commit_message>
<xml_diff>
--- a/Output/AMZReview43APro.xlsx
+++ b/Output/AMZReview43APro.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="193">
   <si>
     <t>Review</t>
   </si>
@@ -129,16 +129,16 @@
     <t>kamal Bharathi</t>
   </si>
   <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Style Name: Google X Series 2024Size: 50</t>
+  </si>
+  <si>
+    <t>Shashi Kant</t>
+  </si>
+  <si>
     <t>Very good ?? ?? percent</t>
-  </si>
-  <si>
-    <t>Shashi Kant</t>
-  </si>
-  <si>
-    <t>Good</t>
-  </si>
-  <si>
-    <t>Style Name: Google X Series 2024Size: 50</t>
   </si>
   <si>
     <t>Amazon Customer</t>
@@ -183,13 +183,16 @@
     <t>Style Name: Google X Series 2023Size: 55</t>
   </si>
   <si>
+    <t>Very good</t>
+  </si>
+  <si>
+    <t>Arslan khan</t>
+  </si>
+  <si>
     <t>It’s good for the price but the sound isn’t so great for “Dolby audio” that’s all. Otherwise all good.</t>
   </si>
   <si>
-    <t>Arslan khan</t>
-  </si>
-  <si>
-    <t>Very good</t>
+    <t>Good product</t>
   </si>
   <si>
     <t>Amazon buyer</t>
@@ -198,25 +201,28 @@
     <t>Value for money</t>
   </si>
   <si>
-    <t>Good product</t>
+    <t>Priye Ranjan Kumar</t>
+  </si>
+  <si>
+    <t>Working well</t>
   </si>
   <si>
     <t>Pranay</t>
   </si>
   <si>
-    <t>Working well</t>
-  </si>
-  <si>
-    <t>Priye Ranjan Kumar</t>
-  </si>
-  <si>
     <t>best video quality good picture quality in this price range good performance</t>
   </si>
   <si>
     <t>Arvind dabhi</t>
   </si>
   <si>
+    <t>Best quality</t>
+  </si>
+  <si>
     <t>Performance is low, quality is good</t>
+  </si>
+  <si>
+    <t>manoj</t>
   </si>
   <si>
     <t>Loved It, i kind of believe processing of external media needs improvement, but that can be fixed with software update (hope so),
@@ -228,16 +234,10 @@
     <t>srinivasa m.</t>
   </si>
   <si>
-    <t>Best quality</t>
+    <t>The tv was good working perfectly fine. But the demo of how the tv works wasn't given properly by the delivery boy,And he delivery boy was arrogant.Overall the product was good but the delivery service wasn't good.The tv promised the ott apps and other features which were in the tv.</t>
   </si>
   <si>
     <t>Baljeet Kaur</t>
-  </si>
-  <si>
-    <t>The picture quality and sound quality is superb and the installation service is also good. However, I am not happy with the delivery. The delivery person refused to deliver to the location and behaved very rudely. He was demanding extra money for the delivery.</t>
-  </si>
-  <si>
-    <t>Style Name: Google X Series 2024Size: 55</t>
   </si>
   <si>
     <t>I have purchased this TV recently during the amazone sale and delivery and installation is also very fast and good by the team. I have very moderate usage of TV and also TV sound and picture quality is also good as per the price segment.
@@ -247,16 +247,16 @@
 Any one have any idea or same issue then pl give your opinion/feedback.</t>
   </si>
   <si>
-    <t>manoj</t>
+    <t>Style Name: Google X Series 2024Size: 55</t>
+  </si>
+  <si>
+    <t>The picture quality and sound quality is superb and the installation service is also good. However, I am not happy with the delivery. The delivery person refused to deliver to the location and behaved very rudely. He was demanding extra money for the delivery.</t>
+  </si>
+  <si>
+    <t>Sridevi</t>
   </si>
   <si>
     <t>Sound balancing is very poor</t>
-  </si>
-  <si>
-    <t>Sarwan Kumar</t>
-  </si>
-  <si>
-    <t>The tv was good working perfectly fine. But the demo of how the tv works wasn't given properly by the delivery boy,And he delivery boy was arrogant.Overall the product was good but the delivery service wasn't good.The tv promised the ott apps and other features which were in the tv.</t>
   </si>
   <si>
     <t>Bhavik Patel</t>
@@ -266,13 +266,13 @@
 Software also smooth and almost lag free</t>
   </si>
   <si>
+    <t>Sarwan Kumar</t>
+  </si>
+  <si>
+    <t>Picture quality, build quality, everything is good except sound quality. Build in speakers are very worst, you have buy a external speaker if want to hear contents clearly</t>
+  </si>
+  <si>
     <t>@runsiva</t>
-  </si>
-  <si>
-    <t>Picture quality, build quality, everything is good except sound quality. Build in speakers are very worst, you have buy a external speaker if want to hear contents clearly</t>
-  </si>
-  <si>
-    <t>Sridevi</t>
   </si>
   <si>
     <t>Sound is good
@@ -282,38 +282,29 @@
     <t>Peddireddy malla Reddy</t>
   </si>
   <si>
+    <t>in this price range this tv is very good. Worth it for buying but there is only one con I noticed in 1 week is Black of this tv not that but no worries its a 27k tv and it works at its best</t>
+  </si>
+  <si>
     <t>Good product at low price</t>
   </si>
   <si>
     <t>pradeep s</t>
   </si>
   <si>
+    <t>The quality is Ok. A 500 rupees installation fee was charged for the wall mount stand.</t>
+  </si>
+  <si>
+    <t>Ravi</t>
+  </si>
+  <si>
     <t>I have booked 2gb Ram and 8gb Rom but I have received in this tv only 4Gb Storage Rest everything okay</t>
   </si>
   <si>
     <t>narayana av</t>
   </si>
   <si>
-    <t>in this price range this tv is very good. Worth it for buying but there is only one con I noticed in 1 week is Black of this tv not that but no worries its a 27k tv and it works at its best</t>
-  </si>
-  <si>
-    <t>The quality is Ok. A 500 rupees installation fee was charged for the wall mount stand.</t>
-  </si>
-  <si>
-    <t>Ravi</t>
-  </si>
-  <si>
-    <t>TV is good in this range. It will become a bit slow but not that much.
-Sound is not upto the mark
-Picture quality is good.
-Installation service was good
-I will give it 4 stars.</t>
-  </si>
-  <si>
-    <t>Rahul</t>
-  </si>
-  <si>
-    <t>Xiaomi A Pro 4k 43 inches
+    <t>Click to play video
+Xiaomi A Pro 4k 43 inches
 Best TV under this budget
 I didn’t expected this much Great quality from a budget segment TV.
 Colours are very crisp and clear.
@@ -333,25 +324,35 @@
 Rest everything is good. Its being just 1st day I am using it so yeah best of luck to me ✌??..</t>
   </si>
   <si>
+    <t>TV is good in this range. It will become a bit slow but not that much.
+Sound is not upto the mark
+Picture quality is good.
+Installation service was good
+I will give it 4 stars.</t>
+  </si>
+  <si>
+    <t>HV</t>
+  </si>
+  <si>
+    <t>Ok but it gets stuck in between while watching look n price is very worth</t>
+  </si>
+  <si>
+    <t>Rahul</t>
+  </si>
+  <si>
+    <t>Good quality but sound very low</t>
+  </si>
+  <si>
+    <t>waseem231986</t>
+  </si>
+  <si>
     <t>Quality is good and sounds also too good ??</t>
   </si>
   <si>
-    <t>HV</t>
-  </si>
-  <si>
-    <t>Ok but it gets stuck in between while watching look n price is very worth</t>
-  </si>
-  <si>
     <t>Pradeep kavali</t>
   </si>
   <si>
     <t>Picture quality is good but sound quality is really bad.</t>
-  </si>
-  <si>
-    <t>TV IS GOOD BUT REMOTE LAG TOO MUCH</t>
-  </si>
-  <si>
-    <t>Mudassir</t>
   </si>
   <si>
     <t>This tv was delivered to me and I have been using it from two days.
@@ -365,9 +366,6 @@
 There is a lot to explore and will post it later once I discover over coming days.</t>
   </si>
   <si>
-    <t>Arun Ramesha</t>
-  </si>
-  <si>
     <t>This review covers about misleading warranty claim, issues with screen mirroring and latency in TalkBack(screen reading software for visually impaired)
 1. The 2 year extended warranty is basically a insurance policy given to us as an OPTION by a insurance company like Zopper and many others. This policy value is capped at 85% of sum of the insured value (which is the tv cost) after depreciation but in the description it says you can claim multiple times as if there is no restrictions at all. This policy becomes null and void once your claim reaches the limit and it doesn't cover the cost of your claim if it is caused by electric fluctuations and physical dents or damages.
 This warranty is absolutely unnecessary since the company itself (Xiaomi) provides 2 year tv panel warranty so, don't get fooled by this absurd description
@@ -376,22 +374,22 @@
 4. TalkBack feature is very hard to use since the voice response has latency and generally the tv user interface is not friendly to use for visually impaired persons.</t>
   </si>
   <si>
-    <t>Good product but from the price (25k) which i bought this TV, there are better products now in 2024 sadly i was a week early on buying this or else would've def not buyed this</t>
+    <t>Arun Ramesha</t>
+  </si>
+  <si>
+    <t>TV IS GOOD BUT REMOTE LAG TOO MUCH</t>
+  </si>
+  <si>
+    <t>TV is good, sound &amp; picutre quality superb but lower storage, It have 8GB ROM but 500 MB RAM is only available to use. I try to attached Pendrive , tv is also not support and tb is hanging after attached 128GB pendrive into TV. I am disappoint with low storage.</t>
   </si>
   <si>
     <t>S.Muruganandam</t>
   </si>
   <si>
-    <t>TV is good, sound &amp; picutre quality superb but lower storage, It have 8GB ROM but 500 MB RAM is only available to use. I try to attached Pendrive , tv is also not support and tb is hanging after attached 128GB pendrive into TV. I am disappoint with low storage.</t>
-  </si>
-  <si>
-    <t>VINAYAKAN K S</t>
-  </si>
-  <si>
     <t>For product Mentioned Premium "Metal" Bezel Less Design nut there is no metal fo Bezels.</t>
   </si>
   <si>
-    <t>Manoj</t>
+    <t>Mudassir</t>
   </si>
   <si>
     <t>pros:
@@ -410,22 +408,22 @@
 2. storage can be increased</t>
   </si>
   <si>
+    <t>Manoj</t>
+  </si>
+  <si>
+    <t>Display is so good but you have to change in settings for your likings, and the sound is the real bummer I had a tv with 20w speakers but they sounded way better than this because it had Dolby atmos, this 30w speakers okish not as expected, the remote is missing a mute feature so my father is having hard time muting the tv because double pressing volume down mutes the tv. And i really suggest you to go for this tv only when you have a home theatre setup or soundbar. And also the viewing angle is not the best you are able see the picture from side but it is greyed out and the brightness is drastically changes when your straight and side so normally tv comes with higher brightness setting which I didn't like so changed it now it looks good but not from side.</t>
+  </si>
+  <si>
     <t>vaishnavi</t>
   </si>
   <si>
-    <t>Display is so good but you have to change in settings for your likings, and the sound is the real bummer I had a tv with 20w speakers but they sounded way better than this because it had Dolby atmos, this 30w speakers okish not as expected, the remote is missing a mute feature so my father is having hard time muting the tv because double pressing volume down mutes the tv. And i really suggest you to go for this tv only when you have a home theatre setup or soundbar. And also the viewing angle is not the best you are able see the picture from side but it is greyed out and the brightness is drastically changes when your straight and side so normally tv comes with higher brightness setting which I didn't like so changed it now it looks good but not from side.</t>
-  </si>
-  <si>
     <t>Wonderful product</t>
   </si>
   <si>
-    <t>Prathamesh Lokhande</t>
-  </si>
-  <si>
-    <t>This TV lacking of Good Sound Quality with Base, and sound mode</t>
-  </si>
-  <si>
-    <t>Sagee</t>
+    <t>Good product but from the price (25k) which i bought this TV, there are better products now in 2024 sadly i was a week early on buying this or else would've def not buyed this</t>
+  </si>
+  <si>
+    <t>VINAYAKAN K S</t>
   </si>
   <si>
     <t>Nice</t>
@@ -434,12 +432,6 @@
     <t>Priyanka</t>
   </si>
   <si>
-    <t>I choosed a wrong platform to order.</t>
-  </si>
-  <si>
-    <t>Bishnuyasha Dash</t>
-  </si>
-  <si>
     <t>Using this product for more than a month. Outstanding product . Value for money. Useless installation service . Third grade installation service .</t>
   </si>
   <si>
@@ -447,9 +439,6 @@
   </si>
   <si>
     <t>Ajay Chaudhary</t>
-  </si>
-  <si>
-    <t>It has low sound quality</t>
   </si>
   <si>
     <t>Quality very good
@@ -483,20 +472,10 @@
     <t>MD ASHKAR ALI</t>
   </si>
   <si>
+    <t>This TV lacking of Good Sound Quality with Base, and sound mode</t>
+  </si>
+  <si>
     <t>Kankala mamatha</t>
-  </si>
-  <si>
-    <t>GOOD</t>
-  </si>
-  <si>
-    <t>MANTU SHARMA</t>
-  </si>
-  <si>
-    <t>Click to play video
-I have taken this tv 3 months back, I didn't even complete my EMI's for this product but here's comes the first issue, screen is on loop, by contacting technician I came to know it's a software issue and it will 800 rupees, thank God I have taken the extra protection plan other wise I have take this to the customer care centre and I should have pay 800. I don't like to see an issue within 3 months.</t>
-  </si>
-  <si>
-    <t>Srikanth goud</t>
   </si>
   <si>
     <t>Video quality is very good, but the internal storage of 8gb is not sufficient.
@@ -510,10 +489,19 @@
     <t>Avinash K.</t>
   </si>
   <si>
+    <t>I choosed a wrong platform to order.</t>
+  </si>
+  <si>
+    <t>Bishnuyasha Dash</t>
+  </si>
+  <si>
     <t>amazing picture and sound quality, but the remote control quality is pathetic</t>
   </si>
   <si>
     <t>Durga Jyothi Kumar</t>
+  </si>
+  <si>
+    <t>It has low sound quality</t>
   </si>
   <si>
     <t>The bass need to be more in this kind of TV's I didn't like the sound of this tv because bass is not that good. The picture quality is fine but I thought if the storage and ram will be higher at this price it would be best. And MI Installation team came 3rd after tv delivery and after calling so many times. The delivery was on date by Amazon but I think it would come much earlier under a weak. One more think this tv doesn't have patchwall plus I don't know why this is</t>
@@ -565,24 +553,6 @@
     <t>Picture quality good best color is so good but voice quality not good</t>
   </si>
   <si>
-    <t>Shubham Setia</t>
-  </si>
-  <si>
-    <t>This is one of the best in it's price range.
-Pros :
-&gt;Picture Quality is awesome.
-&gt;Sound is loud and crisp.
-&gt;SD channels(Cable channels) are highly rendered and clear.
-&gt;4k experience is on another level (excellent).
-Cons:
-&gt;ROM is quite low. It says 8GB but in reality you will get around 4GB of space with all the pre-installed apps which you need to run the device.
-Conclusion :
-If you are using it for 4-5 OTTs and Live TV then it is a MUST BUY for you.</t>
-  </si>
-  <si>
-    <t>Subhashis Das</t>
-  </si>
-  <si>
     <t>Performance has improved my miles over the previous OLED versions also picture quality and display has improved .
 Installation service was also good and the person promptly suggested settings for best viewing
 Voice recognition is also improved .
@@ -604,6 +574,19 @@
     <t>It was great experience function and quality. Obviously value for money</t>
   </si>
   <si>
+    <t>GOOD</t>
+  </si>
+  <si>
+    <t>MANTU SHARMA</t>
+  </si>
+  <si>
+    <t>Click to play video
+I have taken this tv 3 months back, I didn't even complete my EMI's for this product but here's comes the first issue, screen is on loop, by contacting technician I came to know it's a software issue and it will 800 rupees, thank God I have taken the extra protection plan other wise I have take this to the customer care centre and I should have pay 800. I don't like to see an issue within 3 months.</t>
+  </si>
+  <si>
+    <t>Srikanth goud</t>
+  </si>
+  <si>
     <t>TV was delivered by Amazon on time .... But the After Sale Service by Amazon for TV Installation is simply PATHETIC .... I have been a Prime Member of Amazon Since the beginning but never experienced this kind of POOR Service from Amazon ..... No installation Technician came from Amazon for 4 days even after repeated followups and escalations .... 1st they were saying it is Brand installation and then when I asked for the Mi Service ID they told this Amazon Installation ..... Ultimately I had to book a separate installation from Mi and they did it ..... This is WORST experience ever for me from Amazon .... I would recommend that you book the TV installation from the Brand directly instead of Amazon ..... TV itself seems to be fine in this Price Range ....</t>
   </si>
   <si>
@@ -669,16 +652,10 @@
     <t>Nawnit Gautam</t>
   </si>
   <si>
-    <t>Very good product and good quality of any contains.This unit l purchased from Amazon GIF to October 24 now l am so happy. Thanks Mi coy.</t>
+    <t>Colour and contrast ratio is brilliant amazing picture quality and it support HDMI 2.1 which slightly increase more quality in 4k content speaker's is above average not top notch remote is excellent software is also good based on android 14 which work flawless but some gitter is noticable.</t>
   </si>
   <si>
     <t>sikandar</t>
-  </si>
-  <si>
-    <t>Colour and contrast ratio is brilliant amazing picture quality and it support HDMI 2.1 which slightly increase more quality in 4k content speaker's is above average not top notch remote is excellent software is also good based on android 14 which work flawless but some gitter is noticable.</t>
-  </si>
-  <si>
-    <t>Rustom Ali Ex Army</t>
   </si>
   <si>
     <t>Overall tv is good and budget friendly.
@@ -686,10 +663,13 @@
 Sound is good.</t>
   </si>
   <si>
+    <t>Blue</t>
+  </si>
+  <si>
     <t>I didn't like the sound quality of the TV I expected more from the TV, Treble are on the higher side and bass is very low, but on the other hand it's good according to the price. For suggestions:- You have to use some soundbars or home theatre for better experience.</t>
   </si>
   <si>
-    <t>Sourya Kumar</t>
+    <t>Rishi</t>
   </si>
   <si>
     <t>I liked the picture quality and other features. However I found the sound quality is average.
@@ -697,12 +677,6 @@
   </si>
   <si>
     <t>Dwarkesh</t>
-  </si>
-  <si>
-    <t>Wonderful product and its price in a concessional rate will be required more</t>
-  </si>
-  <si>
-    <t>Margi Ete</t>
   </si>
   <si>
     <t>Remote isn't working after 2 weeks</t>
@@ -720,12 +694,6 @@
     <t>Shubham Topare</t>
   </si>
   <si>
-    <t>Tv is Good but sound quality is not and UI lags while using</t>
-  </si>
-  <si>
-    <t>Pratham Talreja</t>
-  </si>
-  <si>
     <t>I bought it in August 2024 the packaging was good damage on executive delivered the product at my doorstep and the check the product whether it was damage or not then after 2 hours MI service centre technician called me for installation and they reach to my home within 1 hour and installed the product but I have to pay it extra 500 rupees for the Wall mount because the Wall mount was not including in the box but that is okay because the Wall mount brand is also MI, functionality of the product is good picture quality is good enough features of the product is good but the space of internal storage is not enough(only 8gb,free space is about 4gb)it should be 16GB or more for internal memory, installation was very quick and we are using the TV for last 2 month for me it's a good product I got it from Amazon at rupees of 20700 and extra 500 I paid for the Wall mount so basically it was a good deal but after that the TV was sold in great Indian festival at rupees of 17700 so I missed the opportunity to buy the product at a low price of that never mind, the product connectivity is good, picture quality was very good just go for it</t>
   </si>
   <si>
@@ -745,6 +713,25 @@
   </si>
   <si>
     <t>MIZANUR RAHMAN</t>
+  </si>
+  <si>
+    <t>Got my tv in 2 days. Tv display and sound is superb and best in class. Watching youtube videos in 4k 60fps without any lag. However the amazon installation service was pathetic. My time alloted was between 10am - 2pm. But technician didnt came in the time slot, at 4pm evening he called me. So amazon can’t provide installation in the given time slot. Also their technician are liar and cheater. As he asked me 750rs for wall mount stand while it’s clearly mention that stand costs 499rs. My advice would be dont go for amazon installation. Better to ask respective company for installation and demo</t>
+  </si>
+  <si>
+    <t>BHAGWAN SINGH</t>
+  </si>
+  <si>
+    <t>Good Led</t>
+  </si>
+  <si>
+    <t>Dr. nayak</t>
+  </si>
+  <si>
+    <t>I purchased this tv due to launch hype and reasonable price, but the tv lags many times due to low available storage,(8gb, out of which 4 gb is available only)if you install any 5 apps out of these (Netflix, hotstar, jiocinema, Sony LIV,zee5, prime video or MX player) , You will definitely feel the lag switching from one to another, also you need to clear cache all the time yo install or update another app, .
+Sound is also not upto mark, feels like 300 wala speaker sound. Isse better 32 inch ka LG tv ka sound hai</t>
+  </si>
+  <si>
+    <t>Shyam</t>
   </si>
 </sst>
 </file>
@@ -917,21 +904,21 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -942,7 +929,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -973,7 +960,7 @@
         <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
@@ -1032,21 +1019,21 @@
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
         <v>44</v>
-      </c>
-      <c r="B19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="20">
@@ -1054,7 +1041,7 @@
         <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
         <v>10</v>
@@ -1096,7 +1083,7 @@
         <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s">
         <v>10</v>
@@ -1107,10 +1094,10 @@
         <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D24" t="s">
         <v>53</v>
@@ -1121,10 +1108,10 @@
         <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D25" t="s">
         <v>55</v>
@@ -1135,10 +1122,13 @@
         <v>56</v>
       </c>
       <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" t="s">
         <v>57</v>
-      </c>
-      <c r="C26" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="27">
@@ -1146,13 +1136,10 @@
         <v>58</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
         <v>10</v>
-      </c>
-      <c r="D27" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="28">
@@ -1160,10 +1147,10 @@
         <v>60</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D28" t="s">
         <v>61</v>
@@ -1174,7 +1161,7 @@
         <v>62</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C29" t="s">
         <v>19</v>
@@ -1230,41 +1217,41 @@
         <v>70</v>
       </c>
       <c r="B33" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D33" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" t="s">
         <v>72</v>
-      </c>
-      <c r="B34" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" t="s">
         <v>74</v>
-      </c>
-      <c r="B35" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="36">
@@ -1275,7 +1262,7 @@
         <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D36" t="s">
         <v>76</v>
@@ -1286,10 +1273,10 @@
         <v>77</v>
       </c>
       <c r="B37" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D37" t="s">
         <v>78</v>
@@ -1300,24 +1287,24 @@
         <v>79</v>
       </c>
       <c r="B38" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" t="s">
-        <v>80</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" t="s">
         <v>81</v>
-      </c>
-      <c r="B39" t="s">
-        <v>39</v>
-      </c>
-      <c r="C39" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="40">
@@ -1325,10 +1312,10 @@
         <v>82</v>
       </c>
       <c r="B40" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="C40" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D40" t="s">
         <v>83</v>
@@ -1339,10 +1326,10 @@
         <v>84</v>
       </c>
       <c r="B41" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="C41" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D41" t="s">
         <v>85</v>
@@ -1353,27 +1340,24 @@
         <v>86</v>
       </c>
       <c r="B42" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="C42" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D42" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B43" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="C43" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" t="s">
-        <v>88</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44">
@@ -1381,24 +1365,27 @@
         <v>89</v>
       </c>
       <c r="B44" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C44" t="s">
         <v>19</v>
       </c>
       <c r="D44" t="s">
-        <v>90</v>
+        <v>28</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C45" t="s">
         <v>19</v>
+      </c>
+      <c r="D45" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="46">
@@ -1406,18 +1393,15 @@
         <v>92</v>
       </c>
       <c r="B46" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C46" t="s">
         <v>10</v>
-      </c>
-      <c r="D46" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B47" t="s">
         <v>5</v>
@@ -1426,12 +1410,12 @@
         <v>10</v>
       </c>
       <c r="D47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B48" t="s">
         <v>36</v>
@@ -1440,12 +1424,12 @@
         <v>19</v>
       </c>
       <c r="D48" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B49" t="s">
         <v>36</v>
@@ -1454,18 +1438,21 @@
         <v>10</v>
       </c>
       <c r="D49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50" t="s">
         <v>100</v>
-      </c>
-      <c r="B50" t="s">
-        <v>9</v>
-      </c>
-      <c r="C50" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="51">
@@ -1478,27 +1465,24 @@
       <c r="C51" t="s">
         <v>6</v>
       </c>
-      <c r="D51" t="s">
-        <v>102</v>
-      </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52" t="s">
         <v>103</v>
-      </c>
-      <c r="B52" t="s">
-        <v>9</v>
-      </c>
-      <c r="C52" t="s">
-        <v>19</v>
-      </c>
-      <c r="D52" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B53" t="s">
         <v>36</v>
@@ -1507,18 +1491,18 @@
         <v>6</v>
       </c>
       <c r="D53" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" t="s">
         <v>107</v>
       </c>
-      <c r="B54" t="s">
-        <v>9</v>
-      </c>
       <c r="C54" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D54" t="s">
         <v>108</v>
@@ -1529,27 +1513,27 @@
         <v>109</v>
       </c>
       <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" t="s">
         <v>110</v>
-      </c>
-      <c r="C55" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
+        <v>111</v>
+      </c>
+      <c r="B56" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" t="s">
         <v>112</v>
-      </c>
-      <c r="B56" t="s">
-        <v>9</v>
-      </c>
-      <c r="C56" t="s">
-        <v>19</v>
-      </c>
-      <c r="D56" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="57">
@@ -1560,7 +1544,7 @@
         <v>9</v>
       </c>
       <c r="C57" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D57" t="s">
         <v>114</v>
@@ -1571,10 +1555,10 @@
         <v>115</v>
       </c>
       <c r="B58" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C58" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D58" t="s">
         <v>116</v>
@@ -1585,10 +1569,10 @@
         <v>117</v>
       </c>
       <c r="B59" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="C59" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D59" t="s">
         <v>118</v>
@@ -1596,77 +1580,74 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>119</v>
+        <v>24</v>
       </c>
       <c r="B60" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C60" t="s">
-        <v>19</v>
-      </c>
-      <c r="D60" t="s">
-        <v>120</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B61" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="C61" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D61" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="B62" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C62" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D62" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" t="s">
+        <v>19</v>
+      </c>
+      <c r="D63" t="s">
         <v>124</v>
-      </c>
-      <c r="B63" t="s">
-        <v>5</v>
-      </c>
-      <c r="C63" t="s">
-        <v>6</v>
-      </c>
-      <c r="D63" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
+        <v>125</v>
+      </c>
+      <c r="B64" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" t="s">
+        <v>10</v>
+      </c>
+      <c r="D64" t="s">
         <v>126</v>
-      </c>
-      <c r="B64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C64" t="s">
-        <v>19</v>
-      </c>
-      <c r="D64" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B65" t="s">
         <v>9</v>
@@ -1675,26 +1656,26 @@
         <v>19</v>
       </c>
       <c r="D65" t="s">
-        <v>129</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B66" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C66" t="s">
         <v>10</v>
       </c>
       <c r="D66" t="s">
-        <v>131</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B67" t="s">
         <v>9</v>
@@ -1703,149 +1684,146 @@
         <v>10</v>
       </c>
       <c r="D67" t="s">
-        <v>7</v>
+        <v>130</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B68" t="s">
         <v>9</v>
       </c>
       <c r="C68" t="s">
-        <v>10</v>
-      </c>
-      <c r="D68" t="s">
-        <v>134</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B69" t="s">
         <v>9</v>
       </c>
       <c r="C69" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="D69" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B70" t="s">
-        <v>9</v>
+        <v>107</v>
       </c>
       <c r="C70" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D70" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B71" t="s">
-        <v>110</v>
+        <v>9</v>
       </c>
       <c r="C71" t="s">
         <v>6</v>
-      </c>
-      <c r="D71" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B72" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C72" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D72" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B73" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C73" t="s">
         <v>19</v>
       </c>
       <c r="D73" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>144</v>
+        <v>40</v>
       </c>
       <c r="B74" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C74" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D74" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B75" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C75" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D75" t="s">
-        <v>147</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>42</v>
+        <v>143</v>
       </c>
       <c r="B76" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C76" t="s">
         <v>6</v>
       </c>
       <c r="D76" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B77" t="s">
         <v>9</v>
       </c>
       <c r="C77" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D77" t="s">
-        <v>7</v>
+        <v>146</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B78" t="s">
         <v>5</v>
@@ -1854,12 +1832,12 @@
         <v>10</v>
       </c>
       <c r="D78" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B79" t="s">
         <v>9</v>
@@ -1868,12 +1846,12 @@
         <v>10</v>
       </c>
       <c r="D79" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B80" t="s">
         <v>9</v>
@@ -1882,26 +1860,26 @@
         <v>10</v>
       </c>
       <c r="D80" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B81" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C81" t="s">
         <v>10</v>
       </c>
       <c r="D81" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B82" t="s">
         <v>9</v>
@@ -1910,12 +1888,12 @@
         <v>10</v>
       </c>
       <c r="D82" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B83" t="s">
         <v>9</v>
@@ -1924,12 +1902,12 @@
         <v>6</v>
       </c>
       <c r="D83" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B84" t="s">
         <v>36</v>
@@ -1938,12 +1916,12 @@
         <v>6</v>
       </c>
       <c r="D84" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B85" t="s">
         <v>39</v>
@@ -1954,7 +1932,7 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B86" t="s">
         <v>9</v>
@@ -1963,12 +1941,12 @@
         <v>10</v>
       </c>
       <c r="D86" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B87" t="s">
         <v>36</v>
@@ -1977,12 +1955,12 @@
         <v>6</v>
       </c>
       <c r="D87" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B88" t="s">
         <v>9</v>
@@ -1991,12 +1969,12 @@
         <v>10</v>
       </c>
       <c r="D88" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B89" t="s">
         <v>9</v>
@@ -2005,37 +1983,40 @@
         <v>10</v>
       </c>
       <c r="D89" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B90" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="C90" t="s">
         <v>10</v>
       </c>
       <c r="D90" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B91" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="C91" t="s">
         <v>10</v>
+      </c>
+      <c r="D91" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B92" t="s">
         <v>9</v>
@@ -2044,130 +2025,130 @@
         <v>10</v>
       </c>
       <c r="D92" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B93" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C93" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D93" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B94" t="s">
         <v>9</v>
       </c>
       <c r="C94" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D94" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B95" t="s">
         <v>5</v>
       </c>
       <c r="C95" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D95" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B96" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C96" t="s">
-        <v>19</v>
-      </c>
-      <c r="D96" t="s">
-        <v>185</v>
+        <v>10</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B97" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C97" t="s">
         <v>10</v>
       </c>
       <c r="D97" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B98" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C98" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D98" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B99" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C99" t="s">
         <v>10</v>
+      </c>
+      <c r="D99" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B100" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C100" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D100" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B101" t="s">
         <v>9</v>
       </c>
       <c r="C101" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D101" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Profile & ID added in pom.xml
</commit_message>
<xml_diff>
--- a/Output/AMZReview43APro.xlsx
+++ b/Output/AMZReview43APro.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="195">
   <si>
     <t>Review</t>
   </si>
@@ -216,13 +216,7 @@
     <t>Arvind dabhi</t>
   </si>
   <si>
-    <t>Best quality</t>
-  </si>
-  <si>
     <t>Performance is low, quality is good</t>
-  </si>
-  <si>
-    <t>manoj</t>
   </si>
   <si>
     <t>Loved It, i kind of believe processing of external media needs improvement, but that can be fixed with software update (hope so),
@@ -238,6 +232,9 @@
   </si>
   <si>
     <t>Baljeet Kaur</t>
+  </si>
+  <si>
+    <t>Best quality</t>
   </si>
   <si>
     <t>I have purchased this TV recently during the amazone sale and delivery and installation is also very fast and good by the team. I have very moderate usage of TV and also TV sound and picture quality is also good as per the price segment.
@@ -250,10 +247,13 @@
     <t>Style Name: Google X Series 2024Size: 55</t>
   </si>
   <si>
+    <t>Sridevi</t>
+  </si>
+  <si>
     <t>The picture quality and sound quality is superb and the installation service is also good. However, I am not happy with the delivery. The delivery person refused to deliver to the location and behaved very rudely. He was demanding extra money for the delivery.</t>
   </si>
   <si>
-    <t>Sridevi</t>
+    <t>manoj</t>
   </si>
   <si>
     <t>Sound balancing is very poor</t>
@@ -353,6 +353,26 @@
   </si>
   <si>
     <t>Picture quality is good but sound quality is really bad.</t>
+  </si>
+  <si>
+    <t>nyc</t>
+  </si>
+  <si>
+    <t>This review covers about misleading warranty claim, issues with screen mirroring and latency in TalkBack(screen reading software for visually impaired)
+1. The 2 year extended warranty is basically a insurance policy given to us as an OPTION by a insurance company like Zopper and many others. This policy value is capped at 85% of sum of the insured value (which is the tv cost) after depreciation but in the description it says you can claim multiple times as if there is no restrictions at all. This policy becomes null and void once your claim reaches the limit and it doesn't cover the cost of your claim if it is caused by electric fluctuations and physical dents or damages.
+This warranty is absolutely unnecessary since the company itself (Xiaomi) provides 2 year tv panel warranty so, don't get fooled by this absurd description
+2. There is a huge latency when it comes to screen mirroring, it is so much that the video and audio mismatches. It is okay for browsing and just internet surfing but not ideal for entertainment.
+3. There are couple of hidden features that is not said in manual or by installation persons, you need to watch a youtube video to know it
+4. TalkBack feature is very hard to use since the voice response has latency and generally the tv user interface is not friendly to use for visually impaired persons.</t>
+  </si>
+  <si>
+    <t>sonam singh</t>
+  </si>
+  <si>
+    <t>TV IS GOOD BUT REMOTE LAG TOO MUCH</t>
+  </si>
+  <si>
+    <t>S.Muruganandam</t>
   </si>
   <si>
     <t>This tv was delivered to me and I have been using it from two days.
@@ -366,30 +386,16 @@
 There is a lot to explore and will post it later once I discover over coming days.</t>
   </si>
   <si>
-    <t>This review covers about misleading warranty claim, issues with screen mirroring and latency in TalkBack(screen reading software for visually impaired)
-1. The 2 year extended warranty is basically a insurance policy given to us as an OPTION by a insurance company like Zopper and many others. This policy value is capped at 85% of sum of the insured value (which is the tv cost) after depreciation but in the description it says you can claim multiple times as if there is no restrictions at all. This policy becomes null and void once your claim reaches the limit and it doesn't cover the cost of your claim if it is caused by electric fluctuations and physical dents or damages.
-This warranty is absolutely unnecessary since the company itself (Xiaomi) provides 2 year tv panel warranty so, don't get fooled by this absurd description
-2. There is a huge latency when it comes to screen mirroring, it is so much that the video and audio mismatches. It is okay for browsing and just internet surfing but not ideal for entertainment.
-3. There are couple of hidden features that is not said in manual or by installation persons, you need to watch a youtube video to know it
-4. TalkBack feature is very hard to use since the voice response has latency and generally the tv user interface is not friendly to use for visually impaired persons.</t>
+    <t>Mudassir</t>
+  </si>
+  <si>
+    <t>TV is good, sound &amp; picutre quality superb but lower storage, It have 8GB ROM but 500 MB RAM is only available to use. I try to attached Pendrive , tv is also not support and tb is hanging after attached 128GB pendrive into TV. I am disappoint with low storage.</t>
   </si>
   <si>
     <t>Arun Ramesha</t>
   </si>
   <si>
-    <t>TV IS GOOD BUT REMOTE LAG TOO MUCH</t>
-  </si>
-  <si>
-    <t>TV is good, sound &amp; picutre quality superb but lower storage, It have 8GB ROM but 500 MB RAM is only available to use. I try to attached Pendrive , tv is also not support and tb is hanging after attached 128GB pendrive into TV. I am disappoint with low storage.</t>
-  </si>
-  <si>
-    <t>S.Muruganandam</t>
-  </si>
-  <si>
     <t>For product Mentioned Premium "Metal" Bezel Less Design nut there is no metal fo Bezels.</t>
-  </si>
-  <si>
-    <t>Mudassir</t>
   </si>
   <si>
     <t>pros:
@@ -420,6 +426,9 @@
     <t>Wonderful product</t>
   </si>
   <si>
+    <t>Aritra</t>
+  </si>
+  <si>
     <t>Good product but from the price (25k) which i bought this TV, there are better products now in 2024 sadly i was a week early on buying this or else would've def not buyed this</t>
   </si>
   <si>
@@ -475,7 +484,7 @@
     <t>This TV lacking of Good Sound Quality with Base, and sound mode</t>
   </si>
   <si>
-    <t>Kankala mamatha</t>
+    <t>Sagee</t>
   </si>
   <si>
     <t>Video quality is very good, but the internal storage of 8gb is not sufficient.
@@ -553,6 +562,9 @@
     <t>Picture quality good best color is so good but voice quality not good</t>
   </si>
   <si>
+    <t>Shubham Setia</t>
+  </si>
+  <si>
     <t>Performance has improved my miles over the previous OLED versions also picture quality and display has improved .
 Installation service was also good and the person promptly suggested settings for best viewing
 Voice recognition is also improved .
@@ -580,8 +592,7 @@
     <t>MANTU SHARMA</t>
   </si>
   <si>
-    <t>Click to play video
-I have taken this tv 3 months back, I didn't even complete my EMI's for this product but here's comes the first issue, screen is on loop, by contacting technician I came to know it's a software issue and it will 800 rupees, thank God I have taken the extra protection plan other wise I have take this to the customer care centre and I should have pay 800. I don't like to see an issue within 3 months.</t>
+    <t>I have taken this tv 3 months back, I didn't even complete my EMI's for this product but here's comes the first issue, screen is on loop, by contacting technician I came to know it's a software issue and it will 800 rupees, thank God I have taken the extra protection plan other wise I have take this to the customer care centre and I should have pay 800. I don't like to see an issue within 3 months.</t>
   </si>
   <si>
     <t>Srikanth goud</t>
@@ -639,17 +650,11 @@
     <t>Sheetal gupta</t>
   </si>
   <si>
-    <t>Quality is best, picture quality is best installation is easy thanks to Amazon</t>
-  </si>
-  <si>
-    <t>vijay kumar sharma</t>
-  </si>
-  <si>
     <t>Received defective piece on 28th Sep 2024. Totally disappointed ??????.. Installation team from Amazon (TVS) didn't replace the TV with new one. I had raised the request for technician Visit from brand Company through amazon to check the performance of TV.. Finally Xiaomi replaced the defective TV with new one 16th Oct. Kudoos to Xiaomi company and Mi Installation TV..
 About TV.. It's Superb, Picture quality is awesome. I loved it.. Performance of this is top notch.. ??</t>
   </si>
   <si>
-    <t>Nawnit Gautam</t>
+    <t>vijay kumar sharma</t>
   </si>
   <si>
     <t>Colour and contrast ratio is brilliant amazing picture quality and it support HDMI 2.1 which slightly increase more quality in 4k content speaker's is above average not top notch remote is excellent software is also good based on android 14 which work flawless but some gitter is noticable.</t>
@@ -1083,7 +1088,7 @@
         <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
         <v>10</v>
@@ -1097,7 +1102,7 @@
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D24" t="s">
         <v>53</v>
@@ -1108,10 +1113,10 @@
         <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D25" t="s">
         <v>55</v>
@@ -1125,21 +1130,21 @@
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
-      </c>
-      <c r="D26" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" t="s">
         <v>58</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" t="s">
         <v>59</v>
-      </c>
-      <c r="C27" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="28">
@@ -1147,7 +1152,7 @@
         <v>60</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
@@ -1312,7 +1317,7 @@
         <v>82</v>
       </c>
       <c r="B40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C40" t="s">
         <v>19</v>
@@ -1365,10 +1370,10 @@
         <v>89</v>
       </c>
       <c r="B44" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D44" t="s">
         <v>28</v>
@@ -1379,7 +1384,7 @@
         <v>90</v>
       </c>
       <c r="B45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C45" t="s">
         <v>19</v>
@@ -1398,47 +1403,47 @@
       <c r="C46" t="s">
         <v>10</v>
       </c>
+      <c r="D46" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B47" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="C47" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D47" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B48" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D48" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B49" t="s">
         <v>36</v>
       </c>
       <c r="C49" t="s">
-        <v>10</v>
-      </c>
-      <c r="D49" t="s">
-        <v>98</v>
+        <v>19</v>
       </c>
     </row>
     <row r="50">
@@ -1446,7 +1451,7 @@
         <v>99</v>
       </c>
       <c r="B50" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="C50" t="s">
         <v>10</v>
@@ -1460,46 +1465,49 @@
         <v>101</v>
       </c>
       <c r="B51" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C51" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="D51" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B52" t="s">
         <v>5</v>
       </c>
       <c r="C52" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D52" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B53" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="C53" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D53" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B54" t="s">
-        <v>107</v>
+        <v>36</v>
       </c>
       <c r="C54" t="s">
         <v>6</v>
@@ -1513,46 +1521,46 @@
         <v>109</v>
       </c>
       <c r="B55" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="C55" t="s">
         <v>6</v>
       </c>
       <c r="D55" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B56" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C56" t="s">
         <v>6</v>
       </c>
       <c r="D56" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B57" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C57" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D57" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B58" t="s">
         <v>9</v>
@@ -1561,51 +1569,51 @@
         <v>19</v>
       </c>
       <c r="D58" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B59" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="C59" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D59" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>24</v>
+        <v>120</v>
       </c>
       <c r="B60" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="C60" t="s">
         <v>10</v>
+      </c>
+      <c r="D60" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>119</v>
+        <v>24</v>
       </c>
       <c r="B61" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C61" t="s">
-        <v>19</v>
-      </c>
-      <c r="D61" t="s">
-        <v>120</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B62" t="s">
         <v>9</v>
@@ -1614,12 +1622,12 @@
         <v>19</v>
       </c>
       <c r="D62" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B63" t="s">
         <v>9</v>
@@ -1628,46 +1636,46 @@
         <v>19</v>
       </c>
       <c r="D63" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B64" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C64" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D64" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B65" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C65" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D65" t="s">
-        <v>7</v>
+        <v>129</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B66" t="s">
         <v>9</v>
       </c>
       <c r="C66" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D66" t="s">
         <v>7</v>
@@ -1675,7 +1683,7 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B67" t="s">
         <v>9</v>
@@ -1684,174 +1692,177 @@
         <v>10</v>
       </c>
       <c r="D67" t="s">
-        <v>130</v>
+        <v>7</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B68" t="s">
         <v>9</v>
       </c>
       <c r="C68" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="D68" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B69" t="s">
         <v>9</v>
       </c>
       <c r="C69" t="s">
-        <v>10</v>
-      </c>
-      <c r="D69" t="s">
-        <v>133</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B70" t="s">
-        <v>107</v>
+        <v>9</v>
       </c>
       <c r="C70" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D70" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B71" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="C71" t="s">
         <v>6</v>
+      </c>
+      <c r="D71" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B72" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="C72" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D72" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B73" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C73" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D73" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>40</v>
+        <v>143</v>
       </c>
       <c r="B74" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C74" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D74" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>142</v>
+        <v>40</v>
       </c>
       <c r="B75" t="s">
         <v>9</v>
       </c>
       <c r="C75" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D75" t="s">
-        <v>7</v>
+        <v>145</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B76" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C76" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D76" t="s">
-        <v>144</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B77" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C77" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D77" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B78" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C78" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D78" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B79" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C79" t="s">
         <v>10</v>
       </c>
       <c r="D79" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B80" t="s">
         <v>9</v>
@@ -1860,107 +1871,107 @@
         <v>10</v>
       </c>
       <c r="D80" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B81" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="C81" t="s">
         <v>10</v>
       </c>
       <c r="D81" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B82" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="C82" t="s">
         <v>10</v>
       </c>
       <c r="D82" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B83" t="s">
         <v>9</v>
       </c>
       <c r="C83" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D83" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B84" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="C84" t="s">
         <v>6</v>
       </c>
       <c r="D84" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B85" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C85" t="s">
         <v>6</v>
+      </c>
+      <c r="D85" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B86" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="C86" t="s">
-        <v>10</v>
-      </c>
-      <c r="D86" t="s">
-        <v>163</v>
+        <v>6</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B87" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="C87" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D87" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B88" t="s">
         <v>9</v>
@@ -1969,12 +1980,12 @@
         <v>10</v>
       </c>
       <c r="D88" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B89" t="s">
         <v>9</v>
@@ -1983,12 +1994,12 @@
         <v>10</v>
       </c>
       <c r="D89" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B90" t="s">
         <v>36</v>
@@ -1997,12 +2008,12 @@
         <v>10</v>
       </c>
       <c r="D90" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B91" t="s">
         <v>9</v>
@@ -2011,12 +2022,12 @@
         <v>10</v>
       </c>
       <c r="D91" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B92" t="s">
         <v>9</v>
@@ -2025,12 +2036,12 @@
         <v>10</v>
       </c>
       <c r="D92" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B93" t="s">
         <v>5</v>
@@ -2039,12 +2050,12 @@
         <v>19</v>
       </c>
       <c r="D93" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B94" t="s">
         <v>9</v>
@@ -2053,12 +2064,12 @@
         <v>19</v>
       </c>
       <c r="D94" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B95" t="s">
         <v>5</v>
@@ -2067,12 +2078,12 @@
         <v>6</v>
       </c>
       <c r="D95" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B96" t="s">
         <v>5</v>
@@ -2083,7 +2094,7 @@
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B97" t="s">
         <v>5</v>
@@ -2092,12 +2103,12 @@
         <v>10</v>
       </c>
       <c r="D97" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B98" t="s">
         <v>9</v>
@@ -2106,12 +2117,12 @@
         <v>10</v>
       </c>
       <c r="D98" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B99" t="s">
         <v>25</v>
@@ -2120,12 +2131,12 @@
         <v>10</v>
       </c>
       <c r="D99" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B100" t="s">
         <v>9</v>
@@ -2134,12 +2145,12 @@
         <v>6</v>
       </c>
       <c r="D100" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B101" t="s">
         <v>9</v>
@@ -2148,7 +2159,7 @@
         <v>19</v>
       </c>
       <c r="D101" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>